<commit_message>
Update Awal, Dana, Lampiran, Bab IV // albert
semua file lampiran ada di Tambahan+Lampiran dari albert
Cover udah bener, cuma kurang biodata pak dedi
Anggaran dana, Jadwal Kegiatan FIX (Bab IV)
Lampiran2 fix (ati2 pas pindah gambar, caption gambarnya suka pindah2
</commit_message>
<xml_diff>
--- a/anggaran_dana.xlsx
+++ b/anggaran_dana.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>No.</t>
   </si>
@@ -41,81 +41,6 @@
     <t>Jumlah</t>
   </si>
   <si>
-    <t>Bahan Habis Pakai</t>
-  </si>
-  <si>
-    <t>a.       Kertas A4 (4 rim)</t>
-  </si>
-  <si>
-    <t>Rp. 200.000,00</t>
-  </si>
-  <si>
-    <t>b.      Catridge</t>
-  </si>
-  <si>
-    <t>Rp. 1.100.000,00</t>
-  </si>
-  <si>
-    <t>c.       Cetak, fotocopy, dan jilid(7 rangkap)</t>
-  </si>
-  <si>
-    <t>Rp. 250.000,00</t>
-  </si>
-  <si>
-    <t>d.      Materai</t>
-  </si>
-  <si>
-    <t>Rp. 56.000,00</t>
-  </si>
-  <si>
-    <t>e.       CD RW</t>
-  </si>
-  <si>
-    <t>Rp. 20.000,00</t>
-  </si>
-  <si>
-    <t>f.       Memory Card</t>
-  </si>
-  <si>
-    <t>g.      Tiket Masuk</t>
-  </si>
-  <si>
-    <t>Rp. 500.000,00</t>
-  </si>
-  <si>
-    <t>h.      Logistik</t>
-  </si>
-  <si>
-    <t>Rp. 1.000.000,00</t>
-  </si>
-  <si>
-    <t>Rp. 3.326.000,00</t>
-  </si>
-  <si>
-    <t>Biaya Lain-lain</t>
-  </si>
-  <si>
-    <t>a.       Pajak</t>
-  </si>
-  <si>
-    <t>b.      Publikasi Jurnal</t>
-  </si>
-  <si>
-    <t>c.       Seminar</t>
-  </si>
-  <si>
-    <t>d.      Buku Referensi</t>
-  </si>
-  <si>
-    <t>e.       Laporan</t>
-  </si>
-  <si>
-    <t>Rp. 1.250.000,00</t>
-  </si>
-  <si>
-    <t>Jumlah Total</t>
-  </si>
-  <si>
     <t>b.      Raspberry Case</t>
   </si>
   <si>
@@ -161,27 +86,25 @@
     <t>d.      Kabel VGA</t>
   </si>
   <si>
-    <t>e.      Mouse &amp; Keyboard</t>
-  </si>
-  <si>
-    <t>f.       Kabel LAN dan RJ 45 Connector (4pcs)</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>g.      VGA Monitor Acer LED 16 in. P166HQL</t>
   </si>
   <si>
-    <t>h.      SD Card 16 GB</t>
+    <t>f.       Kabel LAN dan RJ 45 Connector (10 m)</t>
+  </si>
+  <si>
+    <t>e.      SD Card 16 GB</t>
+  </si>
+  <si>
+    <t>h.      Mouse &amp; Keyboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;Rp&quot;#,##0.00_);[Red]\(&quot;Rp&quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="_([$Rp-421]* #,##0_);_([$Rp-421]* \(#,##0\);_([$Rp-421]* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -221,10 +144,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" activeCellId="1" sqref="C8:C10 C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,249 +465,138 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
         <v>650000</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
         <v>75000</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3">
         <v>125000</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3">
         <v>25000</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7">
-        <v>180000</v>
+        <v>22</v>
+      </c>
+      <c r="C7" s="3">
+        <v>80000</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>47</v>
+        <v>21</v>
+      </c>
+      <c r="C8" s="3">
+        <v>35000</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3">
         <v>850000</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10">
-        <v>80000</v>
+        <v>23</v>
+      </c>
+      <c r="C10" s="3">
+        <v>180000</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="H11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
+      <c r="C12" s="3">
+        <f>SUM(C3:C10)</f>
+        <v>2020000</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
       <c r="H13" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
       <c r="H14" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="H16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="1">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="1">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="1">
-        <v>450000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="1">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="1">
-        <v>8274000</v>
-      </c>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>